<commit_message>
worken on characteristic tables
</commit_message>
<xml_diff>
--- a/lab2b/tabelas/tabelas comando conversor.xlsx
+++ b/lab2b/tabelas/tabelas comando conversor.xlsx
@@ -4,17 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="5.2.f" sheetId="1" r:id="rId1"/>
+    <sheet name="4.1.1d" sheetId="1" r:id="rId1"/>
+    <sheet name="4.1.2d" sheetId="2" r:id="rId2"/>
+    <sheet name="4.2.1d" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>Vo teórico [V]</t>
   </si>
@@ -309,8 +314,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -325,7 +358,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -401,7 +434,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -416,7 +449,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'5.2.f'!$E$3</c:f>
+              <c:f>'4.1.1d'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -439,7 +472,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'5.2.f'!$D$4:$D$9</c:f>
+              <c:f>'4.1.1d'!$D$4:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -466,27 +499,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'5.2.f'!$E$4:$E$9</c:f>
+              <c:f>'4.1.1d'!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>31.830988618379067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.698716694734337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.8732414637843</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>15.915494309189533</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.849358347367168</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.93662073189215</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.9577471545947667</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9788735772973851</c:v>
+                  <c:v>7.9577471545947702</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0661359618223656</c:v>
+                  <c:v>2.1322719236447312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,7 +531,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'5.2.f'!$F$3</c:f>
+              <c:f>'4.1.1d'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -521,7 +554,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'5.2.f'!$D$4:$D$9</c:f>
+              <c:f>'4.1.1d'!$D$4:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -548,27 +581,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'5.2.f'!$F$4:$F$9</c:f>
+              <c:f>'4.1.1d'!$F$4:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>14.5</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.2</c:v>
+                  <c:v>46.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>37.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.22</c:v>
+                  <c:v>25.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.08</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15</c:v>
+                  <c:v>1.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,11 +617,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="216276360"/>
-        <c:axId val="216138472"/>
+        <c:axId val="255991696"/>
+        <c:axId val="255992088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="216276360"/>
+        <c:axId val="255991696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,10 +661,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216138472"/>
+        <c:crossAx val="255992088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -639,7 +672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216138472"/>
+        <c:axId val="255992088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,10 +720,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216276360"/>
+        <c:crossAx val="255991696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,7 +763,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -760,7 +793,905 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Tensão na carga em função do</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> Ângulo de Disparo </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" baseline="0"/>
+              <a:t>α</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4.1.2d'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo teórico [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'4.1.2d'!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4.1.2d'!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.915494309189533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.849358347367168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.93662073189215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9577471545947667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9788735772973851</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0661359618223656</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4.1.2d'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo experimental [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'4.1.2d'!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4.1.2d'!$F$4:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>31.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="232072720"/>
+        <c:axId val="255992480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="232072720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="255992480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="255992480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="232072720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Tensão na carga em função do</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> Ângulo de Disparo </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" baseline="0"/>
+              <a:t>α</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4.2.1d'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo teórico [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'4.2.1d'!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4.2.1d'!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>31.830988618379067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.698716694734337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.8732414637843</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.915494309189533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9577471545947702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1322719236447312</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4.2.1d'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo experimental [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'4.2.1d'!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4.2.1d'!$F$4:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="553828328"/>
+        <c:axId val="553827936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="553828328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553827936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="553827936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553828328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -811,7 +1742,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1362,8 +3405,82 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1651,19 +3768,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="22.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="22.7265625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1680,7 +3797,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -1703,17 +3820,17 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C4" s="4"/>
       <c r="D4" s="9">
         <v>0</v>
       </c>
       <c r="E4" s="10">
-        <f>(50/(2*PI())*(1+COS(D4*PI()/180)))</f>
-        <v>15.915494309189533</v>
+        <f>(50/(PI())*(1+COS(D4*PI()/180)))</f>
+        <v>31.830988618379067</v>
       </c>
       <c r="F4" s="11">
-        <v>14.5</v>
+        <v>48</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="1"/>
@@ -1727,17 +3844,17 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C5" s="4"/>
       <c r="D5" s="9">
         <v>30</v>
       </c>
       <c r="E5" s="10">
-        <f t="shared" ref="E5:E9" si="0">(50/(2*PI())*(1+COS(D5*PI()/180)))</f>
-        <v>14.849358347367168</v>
+        <f t="shared" ref="E5:E9" si="0">(50/(PI())*(1+COS(D5*PI()/180)))</f>
+        <v>29.698716694734337</v>
       </c>
       <c r="F5" s="11">
-        <v>13.2</v>
+        <v>46.2</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="1"/>
@@ -1751,17 +3868,17 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C6" s="4"/>
       <c r="D6" s="9">
         <v>60</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="0"/>
-        <v>11.93662073189215</v>
+        <v>23.8732414637843</v>
       </c>
       <c r="F6" s="11">
-        <v>11</v>
+        <v>37.9</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="1"/>
@@ -1775,17 +3892,17 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C7" s="4"/>
       <c r="D7" s="9">
         <v>90</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="0"/>
-        <v>7.9577471545947667</v>
+        <v>15.915494309189533</v>
       </c>
       <c r="F7" s="11">
-        <v>6.22</v>
+        <v>25.6</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="1"/>
@@ -1799,17 +3916,17 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C8" s="4"/>
       <c r="D8" s="9">
         <v>120</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="0"/>
-        <v>3.9788735772973851</v>
+        <v>7.9577471545947702</v>
       </c>
       <c r="F8" s="11">
-        <v>2.08</v>
+        <v>12.8</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="1"/>
@@ -1823,17 +3940,17 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="4"/>
       <c r="D9" s="12">
         <v>150</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
-        <v>1.0661359618223656</v>
+        <v>2.1322719236447312</v>
       </c>
       <c r="F9" s="14">
-        <v>0.15</v>
+        <v>1.48</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="1"/>
@@ -1847,7 +3964,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1864,7 +3981,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1881,7 +3998,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1898,7 +4015,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1915,7 +4032,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1932,7 +4049,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1949,7 +4066,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1966,7 +4083,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1983,7 +4100,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2000,7 +4117,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2017,7 +4134,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2034,7 +4151,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2056,4 +4173,826 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:Q21"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="22.7265625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C4" s="4"/>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <f>(50/(2*PI())*(1+COS(D4*PI()/180)))</f>
+        <v>15.915494309189533</v>
+      </c>
+      <c r="F4" s="11">
+        <v>31.9</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C5" s="4"/>
+      <c r="D5" s="9">
+        <v>30</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" ref="E5:E9" si="0">(50/(2*PI())*(1+COS(D5*PI()/180)))</f>
+        <v>14.849358347367168</v>
+      </c>
+      <c r="F5" s="11">
+        <v>26.5</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C6" s="4"/>
+      <c r="D6" s="9">
+        <v>60</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="0"/>
+        <v>11.93662073189215</v>
+      </c>
+      <c r="F6" s="11">
+        <v>19</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C7" s="4"/>
+      <c r="D7" s="9">
+        <v>90</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>7.9577471545947667</v>
+      </c>
+      <c r="F7" s="11">
+        <v>11.2</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C8" s="4"/>
+      <c r="D8" s="9">
+        <v>120</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>3.9788735772973851</v>
+      </c>
+      <c r="F8" s="11">
+        <v>4.7</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="4"/>
+      <c r="D9" s="12">
+        <v>150</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0661359618223656</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:Q21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="23.81640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="22.7265625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C4" s="4"/>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <f>(50/(PI())*(1+COS(D4*PI()/180)))</f>
+        <v>31.830988618379067</v>
+      </c>
+      <c r="F4" s="11">
+        <v>72.7</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C5" s="4"/>
+      <c r="D5" s="9">
+        <v>30</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" ref="E5:E9" si="0">(50/(PI())*(1+COS(D5*PI()/180)))</f>
+        <v>29.698716694734337</v>
+      </c>
+      <c r="F5" s="11">
+        <v>69.8</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C6" s="4"/>
+      <c r="D6" s="9">
+        <v>60</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="0"/>
+        <v>23.8732414637843</v>
+      </c>
+      <c r="F6" s="11">
+        <v>53.2</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C7" s="4"/>
+      <c r="D7" s="9">
+        <v>90</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>15.915494309189533</v>
+      </c>
+      <c r="F7" s="11">
+        <v>39.5</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C8" s="4"/>
+      <c r="D8" s="9">
+        <v>120</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>7.9577471545947702</v>
+      </c>
+      <c r="F8" s="11">
+        <v>18.3</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="4"/>
+      <c r="D9" s="12">
+        <v>150</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>2.1322719236447312</v>
+      </c>
+      <c r="F9" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes in excel file 2b
</commit_message>
<xml_diff>
--- a/lab2b/tabelas/tabelas comando conversor.xlsx
+++ b/lab2b/tabelas/tabelas comando conversor.xlsx
@@ -408,7 +408,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -617,11 +616,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="255991696"/>
-        <c:axId val="255992088"/>
+        <c:axId val="395109776"/>
+        <c:axId val="395110952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="255991696"/>
+        <c:axId val="395109776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255992088"/>
+        <c:crossAx val="395110952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -672,7 +671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="255992088"/>
+        <c:axId val="395110952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +722,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255991696"/>
+        <c:crossAx val="395109776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -737,7 +736,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1066,11 +1064,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="232072720"/>
-        <c:axId val="255992480"/>
+        <c:axId val="214089440"/>
+        <c:axId val="214086696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="232072720"/>
+        <c:axId val="214089440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255992480"/>
+        <c:crossAx val="214086696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1121,7 +1119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="255992480"/>
+        <c:axId val="214086696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,7 +1170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232072720"/>
+        <c:crossAx val="214089440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1515,11 +1513,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="553828328"/>
-        <c:axId val="553827936"/>
+        <c:axId val="476612976"/>
+        <c:axId val="476614152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="553828328"/>
+        <c:axId val="476612976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,7 +1560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553827936"/>
+        <c:crossAx val="476614152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1570,7 +1568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553827936"/>
+        <c:axId val="476614152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553828328"/>
+        <c:crossAx val="476612976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4590,8 +4588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4767,7 +4765,7 @@
       <c r="D9" s="12">
         <v>150</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>2.1322719236447312</v>
       </c>

</xml_diff>